<commit_message>
Update Car Inventory pivot table.xlsx
</commit_message>
<xml_diff>
--- a/Car Inventory pivot table.xlsx
+++ b/Car Inventory pivot table.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\GitHub\Pivot-Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CE02DA-CD55-4F56-B5FA-830069F9B18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841A2138-24CA-46B7-BAA8-6F7D5D7F7222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11415" yWindow="105" windowWidth="16530" windowHeight="12135" activeTab="3" xr2:uid="{8DDC7C5A-E9EA-4E0E-924E-C90D51B528B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8DDC7C5A-E9EA-4E0E-924E-C90D51B528B4}"/>
   </bookViews>
   <sheets>
-    <sheet name="count by make &amp; model" sheetId="3" r:id="rId1"/>
-    <sheet name="profit margin by makes" sheetId="4" r:id="rId2"/>
-    <sheet name="average cost of models" sheetId="5" r:id="rId3"/>
-    <sheet name="percentage by color" sheetId="2" r:id="rId4"/>
-    <sheet name="Car Inventory" sheetId="1" r:id="rId5"/>
+    <sheet name="Car Inventory" sheetId="1" r:id="rId1"/>
+    <sheet name="count by make &amp; model" sheetId="3" r:id="rId2"/>
+    <sheet name="profit margin by makes" sheetId="4" r:id="rId3"/>
+    <sheet name="average cost of makes" sheetId="5" r:id="rId4"/>
+    <sheet name="percentage by color" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="42">
   <si>
     <t>Row Labels</t>
   </si>
@@ -247,18 +247,24 @@
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -287,7 +293,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Car Inventory.xlsx]percentage by color!PivotTable2</c:name>
+    <c:name>[Car Inventory pivot table.xlsx]percentage by color!PivotTable2</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -411,54 +417,142 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>'percentage by color'!$A$4:$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Chevrolet</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Dodge</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Ford</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Honda</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Nissan</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Toyota</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:multiLvlStrRef>
+              <c:f>'percentage by color'!$A$4:$A$27</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="17"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>White</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Green</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Silver</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Silver</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Black</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Black</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Silver</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Red</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Blue</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Silver</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>White</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Red</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Green</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Red</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Black</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>Silver</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Blue</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Chevrolet</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Dodge</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Ford</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Honda</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Nissan</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Toyota</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'percentage by color'!$B$4:$B$10</c:f>
+              <c:f>'percentage by color'!$B$4:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.16666666666666666</c:v>
+                  <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4.1666666666666664E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.1666666666666664E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.3333333333333329E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1666666666666664E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.125</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.20833333333333334</c:v>
+                <c:pt idx="6">
+                  <c:v>4.1666666666666664E-2</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.20833333333333334</c:v>
+                <c:pt idx="7">
+                  <c:v>4.1666666666666664E-2</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.125</c:v>
+                <c:pt idx="8">
+                  <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.16666666666666666</c:v>
+                <c:pt idx="9">
+                  <c:v>4.1666666666666664E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.1666666666666664E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.1666666666666664E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.3333333333333329E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.1666666666666664E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.3333333333333329E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.1666666666666664E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.1666666666666664E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1534,7 +1628,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6F01E1E6-FC42-4204-8C19-6C3B0099F005}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6F01E1E6-FC42-4204-8C19-6C3B0099F005}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:H26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -1698,7 +1792,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E9491B2E-8A86-412D-BFE4-C0BB27137984}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E9491B2E-8A86-412D-BFE4-C0BB27137984}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" dataField="1" showAll="0" sortType="descending">
@@ -1790,7 +1884,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B520D2BC-39BF-4621-A867-2BF4B08162C7}" name="PivotTable3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B520D2BC-39BF-4621-A867-2BF4B08162C7}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -1844,10 +1938,10 @@
     <dataField name="Average of Cost" fld="5" subtotal="average" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="2">
+    <format dxfId="5">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="1">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -1864,8 +1958,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F36CD9A0-7F4C-40F7-AB97-F719B0073F0D}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F36CD9A0-7F4C-40F7-AB97-F719B0073F0D}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:B27" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
       <items count="7">
@@ -1898,7 +1992,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" showAll="0" sortType="descending">
+    <pivotField axis="axisRow" dataField="1" showAll="0" sortType="descending">
       <items count="7">
         <item x="3"/>
         <item x="1"/>
@@ -1923,27 +2017,79 @@
     <pivotField numFmtId="164" showAll="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
-  <rowFields count="1">
+  <rowFields count="2">
     <field x="0"/>
+    <field x="2"/>
   </rowFields>
-  <rowItems count="7">
+  <rowItems count="24">
     <i>
       <x/>
     </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
     <i>
       <x v="1"/>
     </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
     <i>
       <x v="2"/>
     </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
     <i>
       <x v="3"/>
     </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
     <i>
       <x v="4"/>
     </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
     <i>
       <x v="5"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
     </i>
     <i t="grand">
       <x/>
@@ -1959,7 +2105,7 @@
     <format dxfId="3">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="0">
+    <format dxfId="2">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -2288,6 +2434,528 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B3CA43-F384-4E3C-853C-EF7ADCDBB550}">
+  <dimension ref="B1:H25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2">
+        <v>63512</v>
+      </c>
+      <c r="F2" s="1">
+        <v>4000</v>
+      </c>
+      <c r="G2" s="1">
+        <v>3000</v>
+      </c>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2">
+        <v>95135</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2500</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2">
+        <v>101354</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2000</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2">
+        <v>75006</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2198</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="2">
+        <v>69847</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3826</v>
+      </c>
+      <c r="G6" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2">
+        <v>55233</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2970</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2">
+        <v>87278</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2224</v>
+      </c>
+      <c r="G8" s="1">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="2">
+        <v>130684</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2798</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="2">
+        <v>59169</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2160</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="2">
+        <v>138789</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2723</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="2">
+        <v>89073</v>
+      </c>
+      <c r="F12" s="1">
+        <v>3950</v>
+      </c>
+      <c r="G12" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="2">
+        <v>109231</v>
+      </c>
+      <c r="F13" s="1">
+        <v>4959</v>
+      </c>
+      <c r="G13" s="1">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="2">
+        <v>87675</v>
+      </c>
+      <c r="F14" s="1">
+        <v>3791</v>
+      </c>
+      <c r="G14" s="1">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="2">
+        <v>140811</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2340</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="2">
+        <v>139300</v>
+      </c>
+      <c r="F16" s="1">
+        <v>3361</v>
+      </c>
+      <c r="G16" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="2">
+        <v>63259</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3196</v>
+      </c>
+      <c r="G17" s="1">
+        <v>3050</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="2">
+        <v>40826</v>
+      </c>
+      <c r="F18" s="1">
+        <v>4397</v>
+      </c>
+      <c r="G18" s="1">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2">
+        <v>41560</v>
+      </c>
+      <c r="F19" s="1">
+        <v>3706</v>
+      </c>
+      <c r="G19" s="1">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="2">
+        <v>49326</v>
+      </c>
+      <c r="F20" s="1">
+        <v>4745</v>
+      </c>
+      <c r="G20" s="1">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="2">
+        <v>101856</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2914</v>
+      </c>
+      <c r="G21" s="1">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="2">
+        <v>42542</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2659</v>
+      </c>
+      <c r="G22" s="1">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="2">
+        <v>34853</v>
+      </c>
+      <c r="F23" s="1">
+        <v>4349</v>
+      </c>
+      <c r="G23" s="1">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="2">
+        <v>58173</v>
+      </c>
+      <c r="F24" s="1">
+        <v>4252</v>
+      </c>
+      <c r="G24" s="1">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="2">
+        <v>136775</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2090</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1800</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA37165D-E37B-4C24-9D69-225DDF784995}">
   <dimension ref="A3:H26"/>
   <sheetViews>
@@ -2744,7 +3412,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F8160A4-69F5-41AA-9FCB-DD2978DABEF5}">
   <dimension ref="A3:E10"/>
   <sheetViews>
@@ -2902,7 +3570,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB809241-DA6C-49A1-97E6-CB7199F5891C}">
   <dimension ref="A3:B10"/>
   <sheetViews>
@@ -2985,12 +3653,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8840E9D9-4C43-4F55-8F1A-810E2D2A56A4}">
-  <dimension ref="A3:B10"/>
+  <dimension ref="A3:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3020,50 +3688,186 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
+      <c r="A5" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="B5" s="9">
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>4</v>
+      <c r="A6" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="B6" s="9">
-        <v>0.20833333333333334</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>5</v>
+      <c r="A7" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="B7" s="9">
-        <v>0.20833333333333334</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8" s="9">
         <v>0.125</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="9">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="9">
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="9">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="9">
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="9">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="9">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="9">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B23" s="9">
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="9">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B27" s="9">
         <v>1</v>
       </c>
     </row>
@@ -3071,526 +3875,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B3CA43-F384-4E3C-853C-EF7ADCDBB550}">
-  <dimension ref="B1:H25"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="2">
-        <v>63512</v>
-      </c>
-      <c r="F2" s="1">
-        <v>4000</v>
-      </c>
-      <c r="G2" s="1">
-        <v>3000</v>
-      </c>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="2">
-        <v>95135</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2500</v>
-      </c>
-      <c r="G3" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="2">
-        <v>101354</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2000</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="2">
-        <v>75006</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2198</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="2">
-        <v>69847</v>
-      </c>
-      <c r="F6" s="1">
-        <v>3826</v>
-      </c>
-      <c r="G6" s="1">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="2">
-        <v>55233</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2970</v>
-      </c>
-      <c r="G7" s="1">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="2">
-        <v>87278</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2224</v>
-      </c>
-      <c r="G8" s="1">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="2">
-        <v>130684</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2798</v>
-      </c>
-      <c r="G9" s="1">
-        <v>2200</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="2">
-        <v>59169</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2160</v>
-      </c>
-      <c r="G10" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="2">
-        <v>138789</v>
-      </c>
-      <c r="F11" s="1">
-        <v>2723</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="2">
-        <v>89073</v>
-      </c>
-      <c r="F12" s="1">
-        <v>3950</v>
-      </c>
-      <c r="G12" s="1">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="2">
-        <v>109231</v>
-      </c>
-      <c r="F13" s="1">
-        <v>4959</v>
-      </c>
-      <c r="G13" s="1">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="2">
-        <v>87675</v>
-      </c>
-      <c r="F14" s="1">
-        <v>3791</v>
-      </c>
-      <c r="G14" s="1">
-        <v>3500</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="2">
-        <v>140811</v>
-      </c>
-      <c r="F15" s="1">
-        <v>2340</v>
-      </c>
-      <c r="G15" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="2">
-        <v>139300</v>
-      </c>
-      <c r="F16" s="1">
-        <v>3361</v>
-      </c>
-      <c r="G16" s="1">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="2">
-        <v>63259</v>
-      </c>
-      <c r="F17" s="1">
-        <v>3196</v>
-      </c>
-      <c r="G17" s="1">
-        <v>3050</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="2">
-        <v>40826</v>
-      </c>
-      <c r="F18" s="1">
-        <v>4397</v>
-      </c>
-      <c r="G18" s="1">
-        <v>3900</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="2">
-        <v>41560</v>
-      </c>
-      <c r="F19" s="1">
-        <v>3706</v>
-      </c>
-      <c r="G19" s="1">
-        <v>3100</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="2">
-        <v>49326</v>
-      </c>
-      <c r="F20" s="1">
-        <v>4745</v>
-      </c>
-      <c r="G20" s="1">
-        <v>4100</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="2">
-        <v>101856</v>
-      </c>
-      <c r="F21" s="1">
-        <v>2914</v>
-      </c>
-      <c r="G21" s="1">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="2">
-        <v>42542</v>
-      </c>
-      <c r="F22" s="1">
-        <v>2659</v>
-      </c>
-      <c r="G22" s="1">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="2">
-        <v>34853</v>
-      </c>
-      <c r="F23" s="1">
-        <v>4349</v>
-      </c>
-      <c r="G23" s="1">
-        <v>3500</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="2">
-        <v>58173</v>
-      </c>
-      <c r="F24" s="1">
-        <v>4252</v>
-      </c>
-      <c r="G24" s="1">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="2">
-        <v>136775</v>
-      </c>
-      <c r="F25" s="1">
-        <v>2090</v>
-      </c>
-      <c r="G25" s="1">
-        <v>1800</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>